<commit_message>
Deploy 3cdaadb from branch develop
</commit_message>
<xml_diff>
--- a/public/AddInfos/en/7.1.2.xlsx
+++ b/public/AddInfos/en/7.1.2.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -139,6 +140,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFCC30B"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -148,6 +154,315 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Population with primary reliance on clean fuels and technology</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:areaChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:noFill/>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>Tabelle2!$A$1:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2016</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle2!$B$1:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>95</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FCC30B"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>Tabelle2!$A$1:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2016</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle2!$C$1:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="45750272"/>
+        <c:axId val="138303104"/>
+      </c:areaChart>
+      <c:catAx>
+        <c:axId val="45750272"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Year</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="138303104"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="138303104"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="100"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Percent (%)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="45750272"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>123824</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>628650</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Diagramm 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -405,7 +720,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -414,10 +729,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:G46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -425,7 +740,7 @@
     <col min="1" max="1" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>3</v>
       </c>
@@ -437,9 +752,8 @@
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
-      <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -451,9 +765,8 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2010</v>
       </c>
@@ -465,9 +778,8 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>2011</v>
       </c>
@@ -479,9 +791,8 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>2012</v>
       </c>
@@ -493,9 +804,8 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>2013</v>
       </c>
@@ -507,9 +817,8 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>2014</v>
       </c>
@@ -521,9 +830,8 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>2015</v>
       </c>
@@ -535,9 +843,8 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>2016</v>
       </c>
@@ -549,9 +856,8 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -559,7 +865,330 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="1"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -567,5 +1196,98 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="3">
+        <v>2010</v>
+      </c>
+      <c r="B1" s="2">
+        <v>95</v>
+      </c>
+      <c r="C1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>2011</v>
+      </c>
+      <c r="B2" s="2">
+        <v>95</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>2012</v>
+      </c>
+      <c r="B3" s="2">
+        <v>95</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>2013</v>
+      </c>
+      <c r="B4" s="2">
+        <v>95</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>2014</v>
+      </c>
+      <c r="B5" s="2">
+        <v>95</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>2015</v>
+      </c>
+      <c r="B6" s="2">
+        <v>95</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>2016</v>
+      </c>
+      <c r="B7" s="2">
+        <v>95</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Deploy 16a2156 from branch develop
</commit_message>
<xml_diff>
--- a/public/AddInfos/en/7.1.2.xlsx
+++ b/public/AddInfos/en/7.1.2.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="7">
   <si>
     <t>&gt; 95</t>
   </si>
@@ -35,6 +35,12 @@
   </si>
   <si>
     <t>Population with primary reliance on clean fuels and technology</t>
+  </si>
+  <si>
+    <t>Datasource:</t>
+  </si>
+  <si>
+    <t>World Health Organization (WHO)</t>
   </si>
 </sst>
 </file>
@@ -339,11 +345,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="45750272"/>
-        <c:axId val="138303104"/>
+        <c:axId val="74814976"/>
+        <c:axId val="41791424"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="45750272"/>
+        <c:axId val="74814976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -373,7 +379,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="138303104"/>
+        <c:crossAx val="41791424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -381,7 +387,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="138303104"/>
+        <c:axId val="41791424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -413,7 +419,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45750272"/>
+        <c:crossAx val="74814976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -720,7 +726,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -732,7 +738,7 @@
   <dimension ref="A1:G46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1047,8 +1053,12 @@
       <c r="G30" s="1"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
+      <c r="A31" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>

</xml_diff>